<commit_message>
updated user story test cases
</commit_message>
<xml_diff>
--- a/Testing/testingScenario.xlsx
+++ b/Testing/testingScenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\priyanka\Git Projects\WorkflowCreator\workFlowCreator\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D482EC7-487F-4C38-84CC-13BDC215E280}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D58767-3C8F-4B6F-9373-55AA2D5E034E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{431FCF67-B4BC-4555-9CF3-EE271EC3F6ED}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="219">
   <si>
     <t>Test Id</t>
   </si>
@@ -569,6 +569,126 @@
   </si>
   <si>
     <t>Cursor pointing should point to newly added shape</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Login page to register user should be available</t>
+  </si>
+  <si>
+    <t>Login page to logged in as registered user</t>
+  </si>
+  <si>
+    <t>On register page option to provide name, username, password and email id is available</t>
+  </si>
+  <si>
+    <t>Verify name fields allows upto 50 characters</t>
+  </si>
+  <si>
+    <t>Verify username fields allows upto 50 characters</t>
+  </si>
+  <si>
+    <t>Verify password is minimum of 15 characters</t>
+  </si>
+  <si>
+    <t>Verfiy password should not start with special characters</t>
+  </si>
+  <si>
+    <t>Verify  Email id is in format XXX@XXX.com</t>
+  </si>
+  <si>
+    <t>Login with the user created above and create the workflows</t>
+  </si>
+  <si>
+    <t>Viewing of the workflow is possible</t>
+  </si>
+  <si>
+    <t>Adding workflow is possible</t>
+  </si>
+  <si>
+    <t>Modifying workflow is possible</t>
+  </si>
+  <si>
+    <t>Deleting the workflow is possible</t>
+  </si>
+  <si>
+    <t>Logged in user name should be displayed on the worklfow screen</t>
+  </si>
+  <si>
+    <t>Logged in user name should be displayed on the mested worklfow screen</t>
+  </si>
+  <si>
+    <t>Create another user and loggin with it. Workflows created by 1st user should not be visible to the 2nd user</t>
+  </si>
+  <si>
+    <t>Logout button should be available</t>
+  </si>
+  <si>
+    <t>TC-083</t>
+  </si>
+  <si>
+    <t>TC-084</t>
+  </si>
+  <si>
+    <t>TC-085</t>
+  </si>
+  <si>
+    <t>TC-086</t>
+  </si>
+  <si>
+    <t>TC-087</t>
+  </si>
+  <si>
+    <t>TC-088</t>
+  </si>
+  <si>
+    <t>TC-089</t>
+  </si>
+  <si>
+    <t>TC-090</t>
+  </si>
+  <si>
+    <t>TC-091</t>
+  </si>
+  <si>
+    <t>TC-092</t>
+  </si>
+  <si>
+    <t>TC-093</t>
+  </si>
+  <si>
+    <t>TC-094</t>
+  </si>
+  <si>
+    <t>TC-095</t>
+  </si>
+  <si>
+    <t>TC-096</t>
+  </si>
+  <si>
+    <t>TC-097</t>
+  </si>
+  <si>
+    <t>TC-098</t>
+  </si>
+  <si>
+    <t>TC-099</t>
+  </si>
+  <si>
+    <t>TC-100</t>
+  </si>
+  <si>
+    <t>On click of the logout user should be navigated back to the login screen</t>
+  </si>
+  <si>
+    <t>User with same username should not be allowed to regsiter</t>
+  </si>
+  <si>
+    <t>TC-101</t>
+  </si>
+  <si>
+    <t>TC-102</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5442C6DF-9EED-412B-A4B9-E0469B0EAB07}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2179,6 +2299,169 @@
       </c>
       <c r="C82" s="10" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B83" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A98" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>